<commit_message>
Trying to modify code to work with heat and light rigs
</commit_message>
<xml_diff>
--- a/flytrack_settings.xlsx
+++ b/flytrack_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonahpearl/Documents/MATLAB/Crickmore/FlyKnight/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FF7C50-FEB4-8E41-AFCE-F8844D65BE39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001526C4-8B3A-414C-A7A3-6BF24FCB0DD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3100" yWindow="2180" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3100" yWindow="2140" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flytrack_settings" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Video direction</t>
   </si>
@@ -89,13 +89,16 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Pixels per cm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -929,18 +932,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -948,7 +951,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -956,7 +959,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -964,7 +967,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -972,7 +975,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -980,7 +983,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -988,7 +991,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -996,7 +999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1004,7 +1007,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1012,7 +1015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1020,7 +1023,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1028,7 +1031,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1036,7 +1039,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1044,7 +1047,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1052,7 +1055,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1060,7 +1063,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1068,7 +1071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1076,12 +1079,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>